<commit_message>
Mise à jours Plesk
</commit_message>
<xml_diff>
--- a/assets/Epreuve-E5/Epreuve E4 - Pago Adrien .xlsx
+++ b/assets/Epreuve-E5/Epreuve E4 - Pago Adrien .xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -138,6 +138,36 @@
       </rPr>
       <t xml:space="preserve"> SISR </t>
     </r>
+  </si>
+  <si>
+    <t>Projet Aide Sociale https://adrien-pago-portfolio.fr/</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Projet Vaca-Meet https://github.com/adrien-pago/Vaca-Meet-Application-Web et https://github.com/adrien-pago/Vaca-Meet-Application-Mobile</t>
+  </si>
+  <si>
+    <t>Du 10/12/22 au 01/03/24</t>
+  </si>
+  <si>
+    <t>Projet GDIN https://adrien-pago-portfolio.fr/</t>
+  </si>
+  <si>
+    <t>du 01/09/23 au 01/10/23</t>
+  </si>
+  <si>
+    <t>portfolio : https://adrien-pago-portfolio.fr/</t>
+  </si>
+  <si>
+    <t>Du 01/01/23 au 01/02/24</t>
+  </si>
+  <si>
+    <t>du 10/01/23 au 27/02/24</t>
   </si>
 </sst>
 </file>
@@ -229,7 +259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -628,46 +658,12 @@
         <color theme="2" tint="-0.749992370372631"/>
       </diagonal>
     </border>
-    <border diagonalUp="1" diagonalDown="1">
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </diagonal>
-    </border>
-    <border diagonalUp="1" diagonalDown="1">
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </diagonal>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -744,15 +740,48 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -777,44 +806,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1127,14 +1126,19 @@
   <dimension ref="A1:AQ81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
-    <col min="3" max="8" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="86.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" style="1" customWidth="1"/>
     <col min="9" max="43" width="11.42578125" customWidth="1"/>
     <col min="44" max="16384" width="10.85546875" style="1"/>
   </cols>
@@ -1166,30 +1170,30 @@
       <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="35" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="36"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="47"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="16" t="s">
         <v>8</v>
       </c>
@@ -1201,22 +1205,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="49"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="35" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1239,8 +1243,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="46"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1296,16 +1300,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="41"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1342,15 +1346,31 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="27"/>
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1388,14 +1408,30 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
+      <c r="A10" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="48" t="s">
+        <v>28</v>
+      </c>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1793,16 +1829,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="44"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1840,14 +1876,30 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="19"/>
+      <c r="A20" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="48" t="s">
+        <v>29</v>
+      </c>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1885,14 +1937,30 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
+      <c r="A21" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="48" t="s">
+        <v>29</v>
+      </c>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1935,7 +2003,7 @@
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="18"/>
       <c r="H22" s="19"/>
       <c r="I22"/>
@@ -2155,16 +2223,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="44"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2202,14 +2270,30 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="27"/>
+      <c r="A28" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2609,6 +2693,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2616,11 +2705,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Update Epreuve E4 - Pago Adrien .xlsx
</commit_message>
<xml_diff>
--- a/assets/Epreuve-E5/Epreuve E4 - Pago Adrien .xlsx
+++ b/assets/Epreuve-E5/Epreuve E4 - Pago Adrien .xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CD47Users\ADPAGO\Documents\GitHub\portfolio\assets\Epreuve-E5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrie\OneDrive\Documents\GitHub\portfolio\assets\Epreuve-E5\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D872925-6D1D-4EFD-8604-855069B5F57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="5760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -143,12 +144,6 @@
     <t>Projet Aide Sociale https://adrien-pago-portfolio.fr/</t>
   </si>
   <si>
-    <t>Oui</t>
-  </si>
-  <si>
-    <t>Non</t>
-  </si>
-  <si>
     <t>Projet Vaca-Meet https://github.com/adrien-pago/Vaca-Meet-Application-Web et https://github.com/adrien-pago/Vaca-Meet-Application-Mobile</t>
   </si>
   <si>
@@ -173,7 +168,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
@@ -663,7 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -671,13 +666,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -686,40 +681,28 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -728,10 +711,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -740,22 +723,31 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -767,10 +759,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -806,18 +798,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Euro" xfId="1"/>
+    <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -833,10 +816,2215 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2351314</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>21772</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>903514</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Connecteur droit 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47B92535-CC5A-1334-73B5-C3A41DFEB7B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8262257" y="8033657"/>
+          <a:ext cx="1578429" cy="881743"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{684162D3-6872-46A2-8F4C-0EFC1ACE4938}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8294914" y="8022771"/>
+          <a:ext cx="1534886" cy="925286"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1502229</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Connecteur droit 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BB8CEB9-42C6-4A2B-B53B-48FA37AF7ABC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11321143" y="8022771"/>
+          <a:ext cx="1491343" cy="936172"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1458686</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Connecteur droit 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{097027E2-AEF8-48E9-BA03-BE32168D2A5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12790715" y="8066314"/>
+          <a:ext cx="1556656" cy="870857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Connecteur droit 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9A2FFF3-7D7A-40F9-9E66-2C7E6416C3A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14347372" y="8055429"/>
+          <a:ext cx="1447799" cy="881742"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Connecteur droit 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{355D0751-BB12-4AE8-B34F-508CD14CEFCB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="15795172" y="8044543"/>
+          <a:ext cx="1523999" cy="892628"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Connecteur droit 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C51B896F-7F83-45A3-B86E-46B313226A03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11342914" y="8011886"/>
+          <a:ext cx="1469572" cy="936171"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1458685</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>206830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1513114</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>914401</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Connecteur droit 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AC7724C-A17F-45D1-925D-98C10CDCE87B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12790714" y="8001001"/>
+          <a:ext cx="1534886" cy="925286"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>914400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Connecteur droit 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{497D3434-9823-48B8-9B86-0ACECC9A6D4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14358256" y="8044544"/>
+          <a:ext cx="1447801" cy="881742"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>32656</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>21773</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Connecteur droit 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3707EAB7-AE71-48F2-86BE-B633C651A301}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15806056" y="8033658"/>
+          <a:ext cx="1534886" cy="925286"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Connecteur droit 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87B8048E-9C12-4ED4-B029-2C1BEE718937}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12823371" y="8937171"/>
+          <a:ext cx="1524000" cy="522515"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1513113</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>914399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>54428</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Connecteur droit 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAC6241C-E6C9-4065-A156-5EB10F92AF8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14325599" y="8926285"/>
+          <a:ext cx="1524000" cy="522515"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>914399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Connecteur droit 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3C1F124-6DFA-497B-BDBB-54FD392F7E99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="15806057" y="8926285"/>
+          <a:ext cx="1524000" cy="522515"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>478972</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Connecteur droit 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A907FF3-0D2E-42F2-8E77-9F6253904524}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12823371" y="8969829"/>
+          <a:ext cx="1513115" cy="446314"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1513114</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>32658</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>468087</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Connecteur droit 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C432BB67-5222-45FC-9796-82A27640C1C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14325600" y="8948057"/>
+          <a:ext cx="1502229" cy="457201"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>21772</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>914400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Connecteur droit 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84CF182F-A4C2-4F8B-BEFE-400FABF3E6C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="15816943" y="8926286"/>
+          <a:ext cx="1502228" cy="511628"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2362200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Connecteur droit 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FA2E67B-151A-479D-8D5E-0EF5491519E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8273143" y="13672457"/>
+          <a:ext cx="1534886" cy="489857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1491342</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Connecteur droit 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D0B9C59-14D6-41B7-99AC-86BB9BE247FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9775371" y="13694229"/>
+          <a:ext cx="1578429" cy="468085"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1469571</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Connecteur droit 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{403B37CA-3DBD-4497-A0D6-8C622FA50DCA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12801600" y="13683343"/>
+          <a:ext cx="1534886" cy="489857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1513114</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>489857</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Connecteur droit 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C806662-FA29-4D40-963F-9AEF18EF9F78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14325600" y="13672457"/>
+          <a:ext cx="1480457" cy="478971"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>489858</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Connecteur droit 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42460887-AA88-4C2A-AB39-C7BDD6161A1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8284029" y="13694229"/>
+          <a:ext cx="1545771" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>10887</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>468087</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Connecteur droit 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B63110D0-9E18-45D6-9810-CFDE1ED2C8D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9808029" y="13672458"/>
+          <a:ext cx="1545771" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>21772</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>21773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>32658</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>478973</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Connecteur droit 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C1D45DF-E192-4201-86EA-8C34BDEC9C71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12834258" y="13683344"/>
+          <a:ext cx="1545771" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>21772</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>489858</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Connecteur droit 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79815943-1237-4EC9-A882-F14A86416FDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14336486" y="13661573"/>
+          <a:ext cx="1480457" cy="489856"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>10887</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>489857</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Connecteur droit 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE9CACEB-574F-4D85-B1FB-A5E2A6629901}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8294915" y="14162314"/>
+          <a:ext cx="1534886" cy="489857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21772</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Connecteur droit 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38F47E22-4A8A-4043-B38D-C1A41D6B4584}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9818915" y="14173200"/>
+          <a:ext cx="1534886" cy="489857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1469571</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Connecteur droit 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCDB5B70-DE99-4B6E-962F-C427BAD9C5CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11342915" y="14173200"/>
+          <a:ext cx="1458685" cy="511629"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1469571</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Connecteur droit 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{851E7883-88FB-411E-B9C2-6B365093EED9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12801600" y="14184086"/>
+          <a:ext cx="1534886" cy="489857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1513114</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>21772</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Connecteur droit 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{136FFA8B-3175-40D2-A4F6-434DE6CB6FE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14325600" y="14184086"/>
+          <a:ext cx="1491343" cy="500743"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>489858</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Connecteur droit 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E46B186-7FC7-4EFF-A260-DBD8959EDB3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14358257" y="14162316"/>
+          <a:ext cx="1480457" cy="489856"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>21772</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Connecteur droit 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56A065A6-AFD4-411D-9909-B2BC08E6E2BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12823371" y="14194971"/>
+          <a:ext cx="1545772" cy="500744"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>500742</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Connecteur droit 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA8F525A-09C0-4B82-97CC-E67F1EA72C4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11332028" y="14173200"/>
+          <a:ext cx="1480457" cy="489856"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1491342</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>21770</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="60" name="Connecteur droit 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85B51A96-F2DA-4F30-9EA9-B886B0CFB3DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9829799" y="14194971"/>
+          <a:ext cx="1480457" cy="489856"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2362199</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>489857</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="Connecteur droit 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EACB6CD-830F-4E8B-8563-933BFBECB5D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8273142" y="14173200"/>
+          <a:ext cx="1556658" cy="478971"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Connecteur droit 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09E6B909-A982-4D5D-A25C-BA600B96FCDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8284029" y="17395371"/>
+          <a:ext cx="1534886" cy="489857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Connecteur droit 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CA943B0-32C4-4C8A-B5DE-E6ECBFC74C96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9808029" y="17395371"/>
+          <a:ext cx="1534886" cy="489857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>32656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>21770</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="65" name="Connecteur droit 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{627F323C-5692-48D0-94B1-6E084D9B4528}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12812487" y="17417142"/>
+          <a:ext cx="1534886" cy="489857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1480458</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>32659</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="Connecteur droit 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1EC858C-27FF-4E23-BF4E-8419ABA5D041}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14292944" y="17395371"/>
+          <a:ext cx="1534886" cy="489857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>21773</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="Connecteur droit 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B74342ED-48D9-4AA1-B07A-CF898DF60B2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="15795173" y="17395371"/>
+          <a:ext cx="1534886" cy="489857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>21773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="Connecteur droit 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBD49D0A-AB25-4E1C-B551-A5C2D75DFE5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15838714" y="17406259"/>
+          <a:ext cx="1480457" cy="489856"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>43544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>54428</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Connecteur droit 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{458400FB-BCD9-4814-A6D9-6B73B0746782}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14369142" y="17428030"/>
+          <a:ext cx="1480457" cy="489856"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>10887</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1502228</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="70" name="Connecteur droit 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B05CCDA-D1F6-4018-9221-0A41E41390B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12834257" y="17395373"/>
+          <a:ext cx="1480457" cy="489856"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>21772</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1502229</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="Connecteur droit 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6CCFA99-7BDC-4E86-924F-058AA0A6B091}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9840686" y="17417144"/>
+          <a:ext cx="1480457" cy="489856"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1480457</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="Connecteur droit 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B80DA479-1762-469E-A073-D1BC9BA919B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8284029" y="17406258"/>
+          <a:ext cx="1480457" cy="489856"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -874,9 +3062,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -911,7 +3099,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -946,7 +3134,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1119,108 +3307,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="86.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" style="1" customWidth="1"/>
-    <col min="9" max="43" width="11.42578125" customWidth="1"/>
-    <col min="44" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="86.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" style="1" customWidth="1"/>
+    <col min="9" max="43" width="11.44140625" customWidth="1"/>
+    <col min="44" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="27"/>
     </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
-    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+    <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="46" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="47"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="46"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
+    <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="16" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
     </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1242,9 +3430,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="36"/>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1299,17 +3487,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1346,31 +3534,19 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="17" t="s">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="B9" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>28</v>
-      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1407,31 +3583,19 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="49" t="s">
-        <v>34</v>
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>32</v>
       </c>
-      <c r="B10" s="50" t="s">
-        <v>35</v>
+      <c r="B10" s="24" t="s">
+        <v>33</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="48" t="s">
-        <v>28</v>
-      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="22"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1468,15 +3632,15 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="19"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1513,15 +3677,15 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="19"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1558,15 +3722,15 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="19"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1603,15 +3767,15 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="19"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1648,15 +3812,15 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="19"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1693,15 +3857,15 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1738,15 +3902,15 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1783,15 +3947,15 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1828,17 +3992,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="32" t="s">
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1875,31 +4039,19 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="49" t="s">
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="50" t="s">
-        <v>36</v>
+      <c r="B20" s="24" t="s">
+        <v>34</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" s="48" t="s">
-        <v>29</v>
-      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="22"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1936,31 +4088,19 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49" t="s">
-        <v>32</v>
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>30</v>
       </c>
-      <c r="B21" s="50" t="s">
-        <v>33</v>
+      <c r="B21" s="24" t="s">
+        <v>31</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>29</v>
-      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="22"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1997,15 +4137,15 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="17"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2042,15 +4182,15 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
       <c r="B23" s="10"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2087,15 +4227,15 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
       <c r="B24" s="10"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="19"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2132,15 +4272,15 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
       <c r="B25" s="10"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="19"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="17"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2177,15 +4317,15 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
       <c r="B26" s="10"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="19"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="17"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2222,17 +4362,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="32" t="s">
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="33"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2269,31 +4409,19 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="49" t="s">
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="50" t="s">
-        <v>36</v>
+      <c r="B28" s="24" t="s">
+        <v>34</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>29</v>
-      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2330,15 +4458,15 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
       <c r="B29" s="10"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="19"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="17"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2375,15 +4503,15 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
       <c r="B30" s="10"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="19"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="17"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2420,15 +4548,15 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
       <c r="B31" s="10"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="19"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="17"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2465,15 +4593,15 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
       <c r="B32" s="10"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="19"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="17"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2510,15 +4638,15 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="21"/>
+    <row r="33" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="17"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2555,15 +4683,15 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="23"/>
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="19"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2600,7 +4728,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -2645,52 +4773,52 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="G1:H1"/>
@@ -2711,5 +4839,6 @@
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="48" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>